<commit_message>
Feathers packs 脚本（未完成） 更新ItemCode
</commit_message>
<xml_diff>
--- a/ItemCodes.xlsx
+++ b/ItemCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\AHKLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BD499A-22AA-4D27-81CE-D93421F4423A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD18BC8C-24CE-4900-B065-FB29CBFF6DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>XP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,10 +45,6 @@
   </si>
   <si>
     <t>10, 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>15, 15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -109,10 +105,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Banker（#FFFF00FA）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Center</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -206,10 +198,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>15, 15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>|&lt;&gt;*71$27.wy1zz00Tzs03zz00Tzk03zy00Dzk01zw00DzU00zw007zU00zw007zU00zw00Dzk01zy00Dzk01zz00Dzy01zzs0TzzkDzzznzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzw</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -220,6 +208,33 @@
   <si>
     <t>|&lt;closeBank&gt;*41$14.00000kAC71nUDk1s0A07U3w1nUsQA300000U</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Banker（NPC #FFFF00FA）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gerrant （NPC #FFFF00FA）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>45, 50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>|&lt;Gerrant&gt;0xFF00FA@1.00$37.A00000900000c00000I1WZ6CCF9X4YZ4sV1mGGEEV99678EQYM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>|&lt;featherPacks&gt;*106$21.z1wy0Tvk00S003s00T003s00D001s20D081s0UD021k08C00Vk02C009U00Q001U00Q003zzzw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feather packs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12, 12</t>
   </si>
 </sst>
 </file>
@@ -904,6 +919,94 @@
         <a:xfrm>
           <a:off x="200025" y="6715125"/>
           <a:ext cx="333333" cy="361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600014</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>352399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="图片 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1765D818-0FC5-11CD-3097-FB8FFFDDA0E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="114300" y="7258050"/>
+          <a:ext cx="485714" cy="209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>542875</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>428577</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="图片 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB6EA54C-6931-8945-CED9-8E8DD707DB71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="142875" y="7620000"/>
+          <a:ext cx="400000" cy="380952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1273,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -1290,13 +1393,13 @@
     <row r="1" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -1307,13 +1410,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1321,10 +1424,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
@@ -1332,160 +1435,186 @@
     </row>
     <row r="4" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="15" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="17" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1609,32 +1738,32 @@
   <sheetData>
     <row r="1" spans="2:4" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="180" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
完善 feather packs 脚本
</commit_message>
<xml_diff>
--- a/ItemCodes.xlsx
+++ b/ItemCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\AHKLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E77082D-E6A1-44F8-B1C4-AC1C6567CCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81A23F8-4DEA-48EA-875A-166B467D4C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1755" yWindow="555" windowWidth="23880" windowHeight="13890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemText" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>XP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -250,6 +250,18 @@
   </si>
   <si>
     <t>60, 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gerrant store</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>270, 230</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>760, 600</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1160,6 +1172,50 @@
         <a:xfrm>
           <a:off x="76200" y="3095625"/>
           <a:ext cx="1584981" cy="1800225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1433843</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC3B7610-0733-0474-8CB6-E76666ACC81E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5334000"/>
+          <a:ext cx="1743075" cy="1081418"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1436,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -1796,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A65E9F8-FAC7-4099-A58C-342A8E6F3CF5}">
   <dimension ref="B1:D116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -1842,7 +1898,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="60" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:4" ht="138" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="5" spans="2:4" ht="60" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:4" ht="60" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:4" ht="60" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
完成 SuperheatItem 脚本 增加ItemCode信息
</commit_message>
<xml_diff>
--- a/ItemCodes.xlsx
+++ b/ItemCodes.xlsx
@@ -8,25 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1_MyProject\AHKLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E817DE57-74E5-474D-B3DE-B520F8D58C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCD1A63-2A0F-41E1-996D-2B551134C930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemText" sheetId="1" r:id="rId1"/>
     <sheet name="View" sheetId="2" r:id="rId2"/>
+    <sheet name="High alching" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
   <si>
     <t>XP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -270,6 +282,54 @@
   </si>
   <si>
     <t>|&lt;tradeGerrant&gt;0xFFFFFF@1.00$36.z000M0A000M0A000M0A000M0ASD1swAQNXNaAMDaNaAMNaNwAMNaNUAMDXsy000000U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iron ore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>|&lt;IronOre&gt;*37$32.3y7zUVwHzk8k5z41A1TV0b0LwEFk5zY4w1TymC0Lzn205zz0U1Dzs80Hzy207DzUUD3js8AUXz2AE8zUQ4270010U000E40004200010U000Dk000000000000000000000008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8, 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6, 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SuperheatSkill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>|&lt;SuperheatSkill&gt;*109$20.zzzxyTjjbrvtxySSTX37sklz48zk0Da06RVVj9yHkTUwDwD3z3wznzzzy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>|&lt;IronBar&gt;*35$28.00y00047000U20040700U03U40010U0045000EjU015zk04jz00Zzw04Uzk0XkT04DsA0Uzw043zy0U7zz403zwU01zo000zU000Q02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IronBar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nature Rune Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Convert Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Value</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -349,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -372,6 +432,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1139,6 +1202,138 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>542873</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>428576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="图片 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D9A2951-B2FE-98E3-699C-A4E2D074957B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123825" y="8982075"/>
+          <a:ext cx="419048" cy="390476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>580965</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>409532</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="图片 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7231562-BD47-147A-D05A-8D7BBECC89DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="104775" y="9467850"/>
+          <a:ext cx="476190" cy="342857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>523829</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>400008</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="图片 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE8C3E4F-43D6-FA23-AC33-492ABD782D2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152400" y="9925050"/>
+          <a:ext cx="371429" cy="333333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1268,6 +1463,759 @@
         <a:xfrm>
           <a:off x="0" y="5334000"/>
           <a:ext cx="1743075" cy="1081418"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1666693</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>361917</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A15CACD-DD26-92CD-BC95-99EF28DC95B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="209550" y="533400"/>
+          <a:ext cx="1457143" cy="266667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1609550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>342868</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCF18952-EB67-A548-A80B-0C2C53ED432B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="209550" y="962025"/>
+          <a:ext cx="1400000" cy="257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1752398</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>352389</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C20B86B5-1D7E-5038-3DE3-B6B85646706C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="1381125"/>
+          <a:ext cx="1619048" cy="285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1552413</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>352389</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E6D4440-0664-BA86-D0B3-E2234B33AD57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="1819275"/>
+          <a:ext cx="1295238" cy="285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1571462</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>361913</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A295AF0C-3378-5DCA-63E0-5F22718513B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="2257425"/>
+          <a:ext cx="1304762" cy="295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1504807</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>390488</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="图片 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69949C26-6977-2583-71F7-35CB1A07ECC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="361950" y="2724150"/>
+          <a:ext cx="1142857" cy="295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1619080</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>380963</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="图片 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B63D397-4139-5B43-6F2A-E9B5E90DEE25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="3152775"/>
+          <a:ext cx="1361905" cy="295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1580989</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>352393</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="图片 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D6D2598-68F5-761C-A9B6-80A319D01680}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="295275" y="3600450"/>
+          <a:ext cx="1285714" cy="257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1542901</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>371436</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="图片 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF40C410-579D-897C-C4CC-76529275C971}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="352425" y="4000500"/>
+          <a:ext cx="1190476" cy="314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1542895</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>361917</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="图片 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{973759B5-0303-F00C-7B4D-E0A8EC1EA636}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="304800" y="4476750"/>
+          <a:ext cx="1238095" cy="266667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1533369</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>390487</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="图片 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0656FCE0-4E87-EE31-315E-CA0DFE4D7DF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="285750" y="4905375"/>
+          <a:ext cx="1247619" cy="304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1514314</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>380964</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="图片 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C41D0DF-BEDE-6270-E9E6-7BD700F1528D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="5353050"/>
+          <a:ext cx="1285714" cy="285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1371473</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>361911</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="图片 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13B74738-E495-E7DD-825C-00D6D2A95137}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="352425" y="5743575"/>
+          <a:ext cx="1019048" cy="314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1495271</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>380957</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="图片 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22FCA800-E5C9-4E7C-1691-2684CA21DB1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="6172200"/>
+          <a:ext cx="1228571" cy="342857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161477</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85606</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="图片 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8DFACCC-0364-692D-99F7-6F63102440F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10039350" y="5267325"/>
+          <a:ext cx="3580952" cy="952381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>275763</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9386</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="图片 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61C81374-89C1-3F62-EB33-CD742D31F51B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10039350" y="4152900"/>
+          <a:ext cx="3695238" cy="1114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>113862</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>209450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="图片 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2BB75F1-ECA4-4991-FD41-09112BAD3773}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10067925" y="3352800"/>
+          <a:ext cx="3504762" cy="800000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1544,8 +2492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -1811,9 +2759,48 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="22" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1917,8 +2904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A65E9F8-FAC7-4099-A58C-342A8E6F3CF5}">
   <dimension ref="B1:D116"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -2091,4 +3078,233 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6728ED06-6CA3-47E0-B3A1-31CDE51A7546}">
+  <dimension ref="A1:D38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="24.875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="27.125" customWidth="1"/>
+    <col min="4" max="4" width="25.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="8">
+        <v>3120</v>
+      </c>
+      <c r="C2" s="8">
+        <v>106</v>
+      </c>
+      <c r="D2" s="8">
+        <f>B2-C2</f>
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="8">
+        <v>4680</v>
+      </c>
+      <c r="C3" s="8">
+        <v>106</v>
+      </c>
+      <c r="D3" s="8">
+        <f t="shared" ref="D3:D15" si="0">B3-C3</f>
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="8">
+        <v>9984</v>
+      </c>
+      <c r="C4" s="8">
+        <v>106</v>
+      </c>
+      <c r="D4" s="8">
+        <f t="shared" si="0"/>
+        <v>9878</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="8">
+        <v>38400</v>
+      </c>
+      <c r="C5" s="8">
+        <v>106</v>
+      </c>
+      <c r="D5" s="8">
+        <f t="shared" si="0"/>
+        <v>38294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="8">
+        <v>32640</v>
+      </c>
+      <c r="C6" s="8">
+        <v>106</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
+        <v>32534</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="8">
+        <v>21120</v>
+      </c>
+      <c r="C7" s="8">
+        <v>106</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="0"/>
+        <v>21014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8">
+        <v>19200</v>
+      </c>
+      <c r="C8" s="8">
+        <v>106</v>
+      </c>
+      <c r="D8" s="8">
+        <f t="shared" si="0"/>
+        <v>19094</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8">
+        <v>30000</v>
+      </c>
+      <c r="C9" s="8">
+        <v>106</v>
+      </c>
+      <c r="D9" s="8">
+        <f t="shared" si="0"/>
+        <v>29894</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8">
+        <v>38400</v>
+      </c>
+      <c r="C10" s="8">
+        <v>106</v>
+      </c>
+      <c r="D10" s="8">
+        <f t="shared" si="0"/>
+        <v>38294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8">
+        <v>23040</v>
+      </c>
+      <c r="C11" s="8">
+        <v>106</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" si="0"/>
+        <v>22934</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="8">
+        <v>38400</v>
+      </c>
+      <c r="C12" s="8">
+        <v>106</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" si="0"/>
+        <v>38294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="8">
+        <v>11520</v>
+      </c>
+      <c r="C13" s="8">
+        <v>106</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" si="0"/>
+        <v>11414</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="8">
+        <v>12480</v>
+      </c>
+      <c r="C14" s="8">
+        <v>106</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="0"/>
+        <v>12374</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="8">
+        <v>19200</v>
+      </c>
+      <c r="C15" s="8">
+        <v>106</v>
+      </c>
+      <c r="D15" s="8">
+        <f t="shared" si="0"/>
+        <v>19094</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
新增： Sammich's OSRS Freemium Bot 样例参考脚本 MakeAttackPotion.ahk MakeGuamPotion.ahk 优化： 库存检测功能
</commit_message>
<xml_diff>
--- a/ItemCodes.xlsx
+++ b/ItemCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1_MyProject\AHKLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2AF5C8-E497-4F4F-B014-05E81158A707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEA791E-AF78-4FF3-B4F4-4C3E0457C930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="87">
   <si>
     <t>Name
 B : Bank Icon
@@ -285,6 +285,38 @@
   </si>
   <si>
     <t>RedSquare</t>
+  </si>
+  <si>
+    <t>VialOfWater</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>|&lt;VialOfWater&gt;*96$21.z1zzwDzzVzzwDzzVzzsDzy1zzk7zw0zzU7zs0zz03zk0Ty03zU0Tw03zU0Dy01zk0DzU3zzUzzzzzU</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GuamLeaf</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>|&lt;GuamLeaf&gt;*41$30.03zzy03zzy0Tzzy1zzzy3zzzw7zzzwDzzzsTzzzsDzzzs3zzzk0zzzk1zzzk3zzzU7zzzUDzzyUDzzfkTzzzUzzzw0Tzz0000000U</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EyeOfNewt</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>|&lt;EyeOfNewt&gt;*123$16.zzzzzzVzwvzbzyDzs3zUDy0zs3zkDzVzzzzzzzzzzzy</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GuamPotion</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>|&lt;GuamPotion&gt;*95$21.z1zzwDzzVzzwDzzVzzsDzz3zzs1zy0DzU1zw0Dz00zk07y00zU03w00TU03y00Dk07zU1zzUTzzzzU</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -440,7 +472,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAAGsBTQEBAAAAAAAAAIADgQKWAQAACAcAAHcBAAB3AQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAAGsBTQEBAAAAAAAAAIADgQKWAQAACAcAAHcBAAB3AQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -497,7 +529,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAACsA6gACAAAAAAAAAJUD7wIdAQAA9wgAAHYCAABnAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAACsA6gACAAAAAAAAAJUD7wIdAQAA9wgAAHYCAABnAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -554,7 +586,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAEAA3gAEAAAAAAAAAKsDvgIOAQAApg4AAEkCAABnAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAEAA3gAEAAAAAAAAAKsDvgIOAQAApg4AAEkCAABnAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -611,7 +643,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAdeF4xHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAGsA9gAFAAAAAAAAAJUDvgIsAQAAlBEAACsCAAA6AgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAdeF4xHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAGsA9gAFAAAAAAAAAJUDvgIsAQAAlBEAACsCAAA6AgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -668,7 +700,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAAJUA6gAGAAAAAAAAAKsDpQIdAQAAghQAABsCAAArAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAAJUA6gAGAAAAAAAAAKsDpQIdAQAAghQAABsCAAArAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -725,7 +757,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAEABQAEHAAAAAAAAAGsDdAKGAQAAyhcAAHcBAACGAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAEABQAEHAAAAAAAAAGsDdAKGAQAAyhcAAHcBAACGAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -782,7 +814,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABcBfRhHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAAABQAEDAAAAAAAAAAADaAKGAQAAXQwAAGgBAABoAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABcBfRhHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAAABQAEDAAAAAAAAAAADaAKGAQAAXQwAAGgBAABoAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -839,7 +871,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACzqnyWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAAIAArAAIAAAAAAAAAIADvgLRAAAAExoAAIYCAAAcAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACzqnyWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAAIAArAAIAAAAAAAAAIADvgLRAAAAExoAAIYCAAAcAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -896,7 +928,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAP18GAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIAAxQAJAAAAAAAAAJUDmQLwAAAA4xwAADoCAAArAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAP18GAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIAAxQAJAAAAAAAAAJUDmQLwAAAA4xwAADoCAAArAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -953,7 +985,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAlrQPyHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAAMAAxQAKAAAAAAAAAKsDTwLwAAAA4B8AAOABAAANAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAlrQPyHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAAMAAxQAKAAAAAAAAAKsDTwLwAAAA4B8AAOABAAANAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1010,7 +1042,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAD/dmMnHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAALUAhwALAAAAAAAAAB4C1wKkAAAA3SIAANECAABoAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAD/dmMnHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAALUAhwALAAAAAAAAAB4C1wKkAAAA3SIAANECAABoAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1067,7 +1099,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC7x/QjHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAAGsBAAAMAAAAAAAAAMACAAQAAAAAJCcAAN8EAADwAAAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC7x/QjHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAAGsBAAAMAAAAAAAAAMACAAQAAAAAJCcAAN8EAADwAAAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1124,7 +1156,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC7rFFzHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAIAAAwENAAAAAAAAAKsDsgI7AQAATykAAA0CAAA6AgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC7rFFzHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAIAAAwENAAAAAAAAAKsDsgI7AQAATykAAA0CAAA6AgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1181,7 +1213,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABcGaBGHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAEABlAAOAAAAAAAAABUDCAO0AAAApiwAAP0CAABKAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABcGaBGHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAEABlAAOAAAAAAAAABUDCAO0AAAApiwAAP0CAABKAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1238,7 +1270,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACZWEwGHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAPAAAAAAAAAGsAuQAPAAAAAAAAAMADvgLhAAAA4C4AAHYCAABYAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACZWEwGHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAPAAAAAAAAAGsAuQAPAAAAAAAAAMADvgLhAAAA4C4AAHYCAABYAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1295,7 +1327,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAsEppRHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAQAAAAAAAAAIABSgAQAAAAAQAAAMACHgFaAAAAczIAAAgIAADhAAAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAsEppRHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAQAAAAAAAAAIABSgAQAAAAAQAAAMACHgFaAAAAczIAAAgIAADhAAAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1352,7 +1384,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAARAAAAAAAAAAABAAARAAAAAQAAAAADWwAAAAAA6TQAAP0FAABoAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAARAAAAAAAAAAABAAARAAAAAQAAAAADWwAAAAAA6TQAAP0FAABoAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1409,7 +1441,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADuWaFyHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAASAAAAAAAAAFUAoAASAAAAAAAAAMADvgLDAAAAQTcAAJQCAABnAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADuWaFyHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAASAAAAAAAAAFUAoAASAAAAAAAAAMADvgLDAAAAQTcAAJQCAABnAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1466,7 +1498,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADQFfAuHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAATAAAAAAAAAJUAhwATAAAAAAAAAJUD7wKkAAAAPjoAAO8CAAAcAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADQFfAuHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAATAAAAAAAAAJUAhwATAAAAAAAAAJUD7wKkAAAAPjoAAO8CAAAcAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1523,7 +1555,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB+7MTBHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAUAAAAAAAAAJUAxQAUAAAAAAAAAIADpQLwAAAADj0AAEgCAAANAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB+7MTBHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAUAAAAAAAAAJUAxQAUAAAAAAAAAIADpQLwAAAADj0AAEgCAAANAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1580,7 +1612,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC//mqwHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAVAAAAAAAAAAAB3gAVAAAAAAAAAFgDEgIOAQAAKUAAAHcBAACmAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC//mqwHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAVAAAAAAAAAAAB3gAVAAAAAAAAAFgDEgIOAQAAKUAAAHcBAACmAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1637,7 +1669,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABe+MbWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAWAAAAAAAAACsB3gAWAAAAAAAAAEADNAIOAQAAF0MAAKEBAAB3AQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABe+MbWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAWAAAAAAAAACsB3gAWAAAAAAAAAEADNAIOAQAAF0MAAKEBAAB3AQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1704,6 +1736,182 @@
         <a:xfrm>
           <a:off x="152400" y="11306174"/>
           <a:ext cx="326448" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>542879</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>419054</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="图片 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{789F4AF7-16E2-68D3-F4F5-B75D27FC2A27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="11734800"/>
+          <a:ext cx="371429" cy="371429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>571452</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>457149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="图片 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40BE8281-C8B6-3FB2-BFC4-ABB48C894C0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="12192000"/>
+          <a:ext cx="380952" cy="409524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533362</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>371436</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="图片 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9F08467-AE2D-9E5D-D524-4E0D2F7E24AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="12658725"/>
+          <a:ext cx="304762" cy="314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>561930</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>428573</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="图片 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4899CE4-22C9-FE02-38B6-B125BF248C56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="200025" y="13068300"/>
+          <a:ext cx="361905" cy="419048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1743,7 +1951,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAACIAjAABAAAAAAAAAMkDwANpAQAA7AQAAEEIAADXDAAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAACIAjAABAAAAAAAAAMkDwANpAQAA7AQAAEEIAADXDAAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1800,7 +2008,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAC0ALwACAAAAAAAAANMD9wN5AAAADBMAAL8JAAARCwAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAC0ALwACAAAAAAAAANMD9wN5AAAADBMAAL8JAAARCwAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1857,7 +2065,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAM4AAAADAAAAAQAAAEYDBgAAAAAA0CAAAF4KAACoBgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAM4AAAADAAAAAQAAAEYDBgAAAAAA0CAAAF4KAACoBgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1919,7 +2127,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABHup1/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAANsAeQABAAAAAAAAAD8DxgNJAQAAVAMAAPkIAACkAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABHup1/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAANsAeQABAAAAAAAAAD8DxgNJAQAAVAMAAPkIAACkAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1976,7 +2184,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAMUAeQACAAAAAAAAABQDpANJAQAAAwYAAJ0IAACVAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAMUAeQACAAAAAAAAABQDpANJAQAAAwYAAJ0IAACVAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2033,7 +2241,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABBk2A5HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAJkATQADAAAAAAAAACoD9wPRAAAAowgAAPcJAADCAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABBk2A5HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAJkATQADAAAAAAAAACoD9wPRAAAAowgAAPcJAADCAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2090,7 +2298,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA8LABCHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAJkAlQAEAAAAAAAAACoDgwOVAQAAYQsAAPcHAADCAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA8LABCHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAJkAlQAEAAAAAAAAACoDgwOVAQAAYQsAAPcHAADCAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2147,7 +2355,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACGNUhOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAJkAmgAFAAAAAAAAAD8DjgOjAQAAHw4AAAcIAADRAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACGNUhOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAJkAmgAFAAAAAAAAAD8DjgOjAQAAHw4AAAcIAADRAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2204,7 +2412,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAANsA0gAGAAAAAAAAAIEDaAM7AgAAChEAAAgHAADRAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAANsA0gAGAAAAAAAAAIEDaAM7AgAAChEAAAgHAADRAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2261,7 +2469,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABdn3JOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAMUAlQAHAAAAAAAAAGsDqgOVAQAAuRMAAGEIAADRAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABdn3JOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAMUAlQAHAAAAAAAAAGsDqgOVAQAAuRMAAGEIAADRAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2318,7 +2526,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB3m21HHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAANsAqwAIAAAAAAAAACoDlAPRAQAAhhYAAOkHAACVAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB3m21HHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAANsAqwAIAAAAAAAAACoDlAPRAQAAhhYAAOkHAACVAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2375,7 +2583,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAsq4VjHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIMAzAAJAAAAAAAAAFUDfgMrAgAACBkAAFQHAADvAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAsq4VjHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIMAzAAJAAAAAAAAAFUDfgMrAgAACBkAAFQHAADvAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2432,7 +2640,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACPhYVuHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAANsAsQAKAAAAAAAAAD8DfgPhAQAAAhwAAJ4HAACkAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACPhYVuHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAANsAsQAKAAAAAAAAAD8DfgPhAQAAAhwAAJ4HAACkAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2489,7 +2697,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAAMUApgALAAAAAAAAAIEDeAPDAQAAsR4AAKsHAADgAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAAMUApgALAAAAAAAAAIEDeAPDAQAAsR4AAKsHAADgAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2546,7 +2754,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA5l2ZBHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAANsAhAAMAAAAAAAAAGsDbQNnAQAAfiEAAOkHAADCAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA5l2ZBHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAANsAhAAMAAAAAAAAAGsDbQNnAQAAfiEAAOkHAADCAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2603,7 +2811,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAG0AzAANAAAAAAAAAD8DGgMrAgAA8SMAAEQGAADvAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAG0AzAANAAAAAAAAAD8DGgMrAgAA8SMAAEQGAADvAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2660,7 +2868,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAFgAmgAOAAAAAAAAAGsDYgOjAQAAoCYAAI8HAAAcAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAFgAmgAOAAAAAAAAAGsDYgOjAQAAoCYAAI8HAAAcAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2717,7 +2925,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADRvqCVHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAABQAAABYADwAOAAAACgAAAMUAAwEUMgAA9yAAAIYUAAD0BQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADRvqCVHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAABQAAABYADwAOAAAACgAAAMUAAwEUMgAA9yAAAIYUAAD0BQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2774,7 +2982,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABGRUBAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAABQAAAOEBDwAMAAAACgAAABYAuwEUMgAA+BkAADoVAAD/BgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABGRUBAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAABQAAAOEBDwAMAAAACgAAABYAuwEUMgAA+BkAADoVAAD/BgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2831,7 +3039,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAABQAAAJACPQAJAAAACgAAAOEBtwBBMgAA9BQAAA4UAAAEBQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAABQAAAJACPQAJAAAACgAAAOEBtwBBMgAA9BQAAA4UAAAEBQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3123,8 +3331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -3466,10 +3674,62 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="29" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add script: CleanGrimyRanarrWeed.ahk MakeRanarrPotion.ahk
</commit_message>
<xml_diff>
--- a/ItemCodes.xlsx
+++ b/ItemCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1_MyProject\AHKLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEA791E-AF78-4FF3-B4F4-4C3E0457C930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6EA958-B9E3-41F9-A041-BA251A8E2128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
   <si>
     <t>Name
 B : Bank Icon
@@ -316,6 +316,26 @@
   </si>
   <si>
     <t>|&lt;GuamPotion&gt;*95$21.z1zzwDzzVzzwDzzVzzsDzz3zzs1zy0DzU1zw0Dz00zk07y00zU03w00TU03y00Dk07zU1zzUTzzzzU</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GrimyRanarrWeed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>|&lt;GrimyRanarrWeed&gt;*37$29.03xzy07rU41zD08DkQ0EzUs13zU02Dxk08sM00Ewy00UTy020Ds040lk083k00UDU010z0021w0027z00sTy0S0Tzz0000002</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RanarrWeed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>|&lt;RanarrWeed&gt;*37$30.03xzy03vk20Tnk21y3U23y3U47w004Dw008Tw008DzU083zk0E0zU0E1XU0E3k00U7k00UDk00UDs00ETw03Uzw0w0Tzz0000000U</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Center</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -472,7 +492,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAAGsBTQEBAAAAAAAAAIADgQKWAQAACAcAAHcBAAB3AQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAAGsBTQEBAAAAAAAAAIADgQKWAQAACAcAAHcBAAB3AQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -529,7 +549,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAACsA6gACAAAAAAAAAJUD7wIdAQAA9wgAAHYCAABnAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAACsA6gACAAAAAAAAAJUD7wIdAQAA9wgAAHYCAABnAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -586,7 +606,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAEAA3gAEAAAAAAAAAKsDvgIOAQAApg4AAEkCAABnAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAEAA3gAEAAAAAAAAAKsDvgIOAQAApg4AAEkCAABnAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -643,7 +663,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAdeF4xHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAGsA9gAFAAAAAAAAAJUDvgIsAQAAlBEAACsCAAA6AgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAdeF4xHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAGsA9gAFAAAAAAAAAJUDvgIsAQAAlBEAACsCAAA6AgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -700,7 +720,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAAJUA6gAGAAAAAAAAAKsDpQIdAQAAghQAABsCAAArAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAAJUA6gAGAAAAAAAAAKsDpQIdAQAAghQAABsCAAArAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -757,7 +777,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAEABQAEHAAAAAAAAAGsDdAKGAQAAyhcAAHcBAACGAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAEABQAEHAAAAAAAAAGsDdAKGAQAAyhcAAHcBAACGAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -814,7 +834,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABcBfRhHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAAABQAEDAAAAAAAAAAADaAKGAQAAXQwAAGgBAABoAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABcBfRhHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAAABQAEDAAAAAAAAAAADaAKGAQAAXQwAAGgBAABoAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -871,7 +891,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACzqnyWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAAIAArAAIAAAAAAAAAIADvgLRAAAAExoAAIYCAAAcAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACzqnyWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAAIAArAAIAAAAAAAAAIADvgLRAAAAExoAAIYCAAAcAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -928,7 +948,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAP18GAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIAAxQAJAAAAAAAAAJUDmQLwAAAA4xwAADoCAAArAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAP18GAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIAAxQAJAAAAAAAAAJUDmQLwAAAA4xwAADoCAAArAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -985,7 +1005,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAlrQPyHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAAMAAxQAKAAAAAAAAAKsDTwLwAAAA4B8AAOABAAANAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAlrQPyHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAAMAAxQAKAAAAAAAAAKsDTwLwAAAA4B8AAOABAAANAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1042,7 +1062,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAD/dmMnHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAALUAhwALAAAAAAAAAB4C1wKkAAAA3SIAANECAABoAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAD/dmMnHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAALUAhwALAAAAAAAAAB4C1wKkAAAA3SIAANECAABoAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1099,7 +1119,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC7x/QjHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAAGsBAAAMAAAAAAAAAMACAAQAAAAAJCcAAN8EAADwAAAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC7x/QjHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAAGsBAAAMAAAAAAAAAMACAAQAAAAAJCcAAN8EAADwAAAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1156,7 +1176,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC7rFFzHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAIAAAwENAAAAAAAAAKsDsgI7AQAATykAAA0CAAA6AgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC7rFFzHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAIAAAwENAAAAAAAAAKsDsgI7AQAATykAAA0CAAA6AgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1213,7 +1233,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABcGaBGHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAEABlAAOAAAAAAAAABUDCAO0AAAApiwAAP0CAABKAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABcGaBGHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAEABlAAOAAAAAAAAABUDCAO0AAAApiwAAP0CAABKAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1270,7 +1290,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACZWEwGHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAPAAAAAAAAAGsAuQAPAAAAAAAAAMADvgLhAAAA4C4AAHYCAABYAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACZWEwGHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAPAAAAAAAAAGsAuQAPAAAAAAAAAMADvgLhAAAA4C4AAHYCAABYAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1327,7 +1347,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAsEppRHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAQAAAAAAAAAIABSgAQAAAAAQAAAMACHgFaAAAAczIAAAgIAADhAAAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAsEppRHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAQAAAAAAAAAIABSgAQAAAAAQAAAMACHgFaAAAAczIAAAgIAADhAAAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1384,7 +1404,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAARAAAAAAAAAAABAAARAAAAAQAAAAADWwAAAAAA6TQAAP0FAABoAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAARAAAAAAAAAAABAAARAAAAAQAAAAADWwAAAAAA6TQAAP0FAABoAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1441,7 +1461,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADuWaFyHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAASAAAAAAAAAFUAoAASAAAAAAAAAMADvgLDAAAAQTcAAJQCAABnAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADuWaFyHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAASAAAAAAAAAFUAoAASAAAAAAAAAMADvgLDAAAAQTcAAJQCAABnAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1498,7 +1518,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADQFfAuHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAATAAAAAAAAAJUAhwATAAAAAAAAAJUD7wKkAAAAPjoAAO8CAAAcAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADQFfAuHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAATAAAAAAAAAJUAhwATAAAAAAAAAJUD7wKkAAAAPjoAAO8CAAAcAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1555,7 +1575,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB+7MTBHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAUAAAAAAAAAJUAxQAUAAAAAAAAAIADpQLwAAAADj0AAEgCAAANAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB+7MTBHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAUAAAAAAAAAJUAxQAUAAAAAAAAAIADpQLwAAAADj0AAEgCAAANAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1612,7 +1632,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC//mqwHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAVAAAAAAAAAAAB3gAVAAAAAAAAAFgDEgIOAQAAKUAAAHcBAACmAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC//mqwHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAVAAAAAAAAAAAB3gAVAAAAAAAAAFgDEgIOAQAAKUAAAHcBAACmAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1669,7 +1689,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABe+MbWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAWAAAAAAAAACsB3gAWAAAAAAAAAEADNAIOAQAAF0MAAKEBAAB3AQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABe+MbWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAWAAAAAAAAACsB3gAWAAAAAAAAAEADNAIOAQAAF0MAAKEBAAB3AQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1912,6 +1932,94 @@
         <a:xfrm>
           <a:off x="200025" y="13068300"/>
           <a:ext cx="361905" cy="419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>542885</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>390489</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="图片 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{891C3CA2-8713-14A8-D40C-7F27036D4642}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="219075" y="13620750"/>
+          <a:ext cx="323810" cy="285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>571458</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>409533</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="图片 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A743E89-9EB0-36D8-604E-6114394321CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="238125" y="14049375"/>
+          <a:ext cx="333333" cy="333333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1951,7 +2059,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAACIAjAABAAAAAAAAAMkDwANpAQAA7AQAAEEIAADXDAAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAACIAjAABAAAAAAAAAMkDwANpAQAA7AQAAEEIAADXDAAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2008,7 +2116,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAC0ALwACAAAAAAAAANMD9wN5AAAADBMAAL8JAAARCwAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAC0ALwACAAAAAAAAANMD9wN5AAAADBMAAL8JAAARCwAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2065,7 +2173,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAM4AAAADAAAAAQAAAEYDBgAAAAAA0CAAAF4KAACoBgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAM4AAAADAAAAAQAAAEYDBgAAAAAA0CAAAF4KAACoBgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2127,7 +2235,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABHup1/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAANsAeQABAAAAAAAAAD8DxgNJAQAAVAMAAPkIAACkAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABHup1/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAANsAeQABAAAAAAAAAD8DxgNJAQAAVAMAAPkIAACkAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2184,7 +2292,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAMUAeQACAAAAAAAAABQDpANJAQAAAwYAAJ0IAACVAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAMUAeQACAAAAAAAAABQDpANJAQAAAwYAAJ0IAACVAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2241,7 +2349,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABBk2A5HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAJkATQADAAAAAAAAACoD9wPRAAAAowgAAPcJAADCAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABBk2A5HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAJkATQADAAAAAAAAACoD9wPRAAAAowgAAPcJAADCAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2298,7 +2406,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA8LABCHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAJkAlQAEAAAAAAAAACoDgwOVAQAAYQsAAPcHAADCAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA8LABCHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAJkAlQAEAAAAAAAAACoDgwOVAQAAYQsAAPcHAADCAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2355,7 +2463,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACGNUhOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAJkAmgAFAAAAAAAAAD8DjgOjAQAAHw4AAAcIAADRAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACGNUhOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAJkAmgAFAAAAAAAAAD8DjgOjAQAAHw4AAAcIAADRAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2412,7 +2520,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAANsA0gAGAAAAAAAAAIEDaAM7AgAAChEAAAgHAADRAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAANsA0gAGAAAAAAAAAIEDaAM7AgAAChEAAAgHAADRAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2469,7 +2577,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABdn3JOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAMUAlQAHAAAAAAAAAGsDqgOVAQAAuRMAAGEIAADRAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABdn3JOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAMUAlQAHAAAAAAAAAGsDqgOVAQAAuRMAAGEIAADRAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2526,7 +2634,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB3m21HHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAANsAqwAIAAAAAAAAACoDlAPRAQAAhhYAAOkHAACVAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB3m21HHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAANsAqwAIAAAAAAAAACoDlAPRAQAAhhYAAOkHAACVAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2583,7 +2691,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAsq4VjHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIMAzAAJAAAAAAAAAFUDfgMrAgAACBkAAFQHAADvAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAsq4VjHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIMAzAAJAAAAAAAAAFUDfgMrAgAACBkAAFQHAADvAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2640,7 +2748,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACPhYVuHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAANsAsQAKAAAAAAAAAD8DfgPhAQAAAhwAAJ4HAACkAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACPhYVuHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAANsAsQAKAAAAAAAAAD8DfgPhAQAAAhwAAJ4HAACkAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2697,7 +2805,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAAMUApgALAAAAAAAAAIEDeAPDAQAAsR4AAKsHAADgAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAAMUApgALAAAAAAAAAIEDeAPDAQAAsR4AAKsHAADgAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2754,7 +2862,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA5l2ZBHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAANsAhAAMAAAAAAAAAGsDbQNnAQAAfiEAAOkHAADCAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA5l2ZBHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAANsAhAAMAAAAAAAAAGsDbQNnAQAAfiEAAOkHAADCAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2811,7 +2919,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAG0AzAANAAAAAAAAAD8DGgMrAgAA8SMAAEQGAADvAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAG0AzAANAAAAAAAAAD8DGgMrAgAA8SMAAEQGAADvAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2868,7 +2976,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAFgAmgAOAAAAAAAAAGsDYgOjAQAAoCYAAI8HAAAcAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAFgAmgAOAAAAAAAAAGsDYgOjAQAAoCYAAI8HAAAcAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2925,7 +3033,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADRvqCVHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAABQAAABYADwAOAAAACgAAAMUAAwEUMgAA9yAAAIYUAAD0BQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADRvqCVHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAABQAAABYADwAOAAAACgAAAMUAAwEUMgAA9yAAAIYUAAD0BQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2982,7 +3090,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABGRUBAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAABQAAAOEBDwAMAAAACgAAABYAuwEUMgAA+BkAADoVAAD/BgAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABGRUBAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAABQAAAOEBDwAMAAAACgAAABYAuwEUMgAA+BkAADoVAAD/BgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3039,7 +3147,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" xmlns="" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAABQAAAJACPQAJAAAACgAAAOEBtwBBMgAA9BQAAA4UAAAEBQAAAQAAAA=="/>
+              <pm:smNativeData xmlns="" xmlns:pm="smNativeData" val="SMDATA_15_NZz4YxMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAABQAAAJACPQAJAAAACgAAAOEBtwBBMgAA9BQAAA4UAAAEBQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3332,7 +3440,7 @@
   <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -3730,8 +3838,34 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="31" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
optimize CleanGrimyRanarrWeed.ahk add script NMZ.ahk
</commit_message>
<xml_diff>
--- a/ItemCodes.xlsx
+++ b/ItemCodes.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <fileSharing readOnlyRecommended="0" userName="Admin"/>
+  <fileSharing readOnlyRecommended="0" userName="A"/>
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
@@ -15,17 +15,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1679812782" val="1060" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1679812782" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1679812782" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1679812782"/>
+      <pm:revision xmlns:pm="smNativeData" day="1680171412" val="1062" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1680171412" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1680171412" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1680171412"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="128">
   <si>
     <t>Name
 B : Bank Icon
@@ -350,6 +350,24 @@
   </si>
   <si>
     <t>|&lt;SandyRocksTag&gt;0xFF00FA@1.00$60.0002000000Q002000080W002000080U002000080QAQCG2X3+C2GGGG34YAE2CGGG24YAAYGGGC24Y+2MCGC22339Q00002000000000G000000000A000000000000000U</t>
+  </si>
+  <si>
+    <t>PurplePixel</t>
+  </si>
+  <si>
+    <t>|&lt;PurplePixel&gt;0xFF00FF@1.00$1.k</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>|&lt;Absorption&gt;##0$0/0/A6933C,4/0/5B5121,0/3/A3903B,4/3/52481D,-2/10/000001,-1/26/A4B1B7,4/26/647E89,-6/25/000001,8/25/000001</t>
+  </si>
+  <si>
+    <t>HPNum1</t>
+  </si>
+  <si>
+    <t>|&lt;HPNum1&gt;0xFF0800@1.00$4.1AF4FC08</t>
   </si>
   <si>
     <t>View</t>
@@ -419,7 +437,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1679812782" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1680171412" ulstyle="none" kern="1">
             <pm:latin face="等线" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -434,7 +452,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1679812782" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1680171412" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -450,7 +468,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1679812782" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1680171412" ulstyle="none" kern="1">
             <pm:latin face="微软雅黑" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -467,7 +485,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1679812782" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1680171412" ulstyle="none" kern="1">
             <pm:latin face="微软雅黑" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -489,7 +507,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1679812782" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1680171412" type="1" fgLvl="100" fgClr="00FFFF00" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -500,7 +518,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1679812782" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1680171412" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -522,7 +540,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1679812782"/>
+          <pm:border xmlns:pm="smNativeData" id="1680171412"/>
         </ext>
       </extLst>
     </border>
@@ -541,7 +559,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1679812782">
+          <pm:border xmlns:pm="smNativeData" id="1680171412">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -565,7 +583,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1679812782"/>
+          <pm:border xmlns:pm="smNativeData" id="1680171412"/>
         </ext>
       </extLst>
     </border>
@@ -606,10 +624,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1679812782" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1680171412" count="1">
         <pm:charStyle name="普通" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1679812782" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1680171412" count="1">
         <pm:color name="黑色" rgb="000000"/>
       </pm:colors>
     </ext>
@@ -634,12 +652,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="43" name="图片 1"/>
+        <xdr:cNvPr id="46" name="图片 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAAGsBTQEBAAAAAAAAAIADgQKWAQAACAcAAHcBAAB3AQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAAGsBTQEBAAAAAAAAAIADgQKWAQAACAcAAHcBAAB3AQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -685,12 +703,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="图片 2"/>
+        <xdr:cNvPr id="45" name="图片 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAACsA6gACAAAAAAAAAJUD7wIdAQAA9wgAAHYCAABnAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAACsA6gACAAAAAAAAAJUD7wIdAQAA9wgAAHYCAABnAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -736,12 +754,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="图片 3"/>
+        <xdr:cNvPr id="44" name="图片 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABBAEEAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAEAA3gAEAAAAAAAAAKsDvgIOAQAApg4AAEkCAABnAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABBAEEAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAEAA3gAEAAAAAAAAAKsDvgIOAQAApg4AAEkCAABnAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -787,12 +805,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="图片 4"/>
+        <xdr:cNvPr id="43" name="图片 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAGsA9gAFAAAAAAAAAJUDvgIsAQAAlBEAACsCAAA6AgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAGsA9gAFAAAAAAAAAJUDvgIsAQAAlBEAACsCAAA6AgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -838,12 +856,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="图片 5"/>
+        <xdr:cNvPr id="42" name="图片 5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAAJUA6gAGAAAAAAAAAKsDpQIdAQAAghQAABsCAAArAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAAJUA6gAGAAAAAAAAAKsDpQIdAQAAghQAABsCAAArAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -889,12 +907,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="图片 6"/>
+        <xdr:cNvPr id="41" name="图片 6"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAdeF4xHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAEABQAEHAAAAAAAAAGsDdAKGAQAAyhcAAHcBAACGAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAdeF4xHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAEABQAEHAAAAAAAAAGsDdAKGAQAAyhcAAHcBAACGAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -940,12 +958,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="图片 7"/>
+        <xdr:cNvPr id="40" name="图片 7"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAAABQAEDAAAAAAAAAAADaAKGAQAAXQwAAGgBAABoAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAAABQAEDAAAAAAAAAAADaAKGAQAAXQwAAGgBAABoAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -991,12 +1009,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="图片 8"/>
+        <xdr:cNvPr id="39" name="图片 8"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABBAEEAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAAIAArAAIAAAAAAAAAIADvgLRAAAAExoAAIYCAAAcAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABBAEEAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAAIAArAAIAAAAAAAAAIADvgLRAAAAExoAAIYCAAAcAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1042,12 +1060,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="图片 9"/>
+        <xdr:cNvPr id="38" name="图片 9"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAcUrMhHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIAAxQAJAAAAAAAAAJUDmQLwAAAA4xwAADoCAAArAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAcUrMhHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIAAxQAJAAAAAAAAAJUDmQLwAAAA4xwAADoCAAArAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1093,12 +1111,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="图片 10"/>
+        <xdr:cNvPr id="37" name="图片 10"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC8fXDwHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAAMAAxQAKAAAAAAAAAKsDTwLwAAAA4B8AAOABAAANAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC8fXDwHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAAMAAxQAKAAAAAAAAAKsDTwLwAAAA4B8AAOABAAANAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1144,12 +1162,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="图片 11"/>
+        <xdr:cNvPr id="36" name="图片 11"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADRt2xeHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAALUAhwALAAAAAAAAAB4C1wKkAAAA3SIAANECAABoAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADRt2xeHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAALUAhwALAAAAAAAAAB4C1wKkAAAA3SIAANECAABoAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1195,12 +1213,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="图片 13"/>
+        <xdr:cNvPr id="35" name="图片 13"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAB2TmTHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAAGsBAAAMAAAAAAAAAMACAAQAAAAAJCcAAN8EAADwAAAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAB2TmTHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAAGsBAAAMAAAAAAAAAMACAAQAAAAAJCcAAN8EAADwAAAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1246,12 +1264,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="图片 12"/>
+        <xdr:cNvPr id="34" name="图片 12"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAUCyYWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAIAAAwENAAAAAAAAAKsDsgI7AQAATykAAA0CAAA6AgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAUCyYWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAIAAAwENAAAAAAAAAKsDsgI7AQAATykAAA0CAAA6AgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1297,12 +1315,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="图片 14"/>
+        <xdr:cNvPr id="33" name="图片 14"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABGhbOdHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAEABlAAOAAAAAAAAABUDCAO0AAAApiwAAP0CAABKAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABGhbOdHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAEABlAAOAAAAAAAAABUDCAO0AAAApiwAAP0CAABKAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1348,12 +1366,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="图片 15"/>
+        <xdr:cNvPr id="32" name="图片 15"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABCRp3PHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAPAAAAAAAAAGsAuQAPAAAAAAAAAMADvgLhAAAA4C4AAHYCAABYAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABCRp3PHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAPAAAAAAAAAGsAuQAPAAAAAAAAAMADvgLhAAAA4C4AAHYCAABYAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1399,12 +1417,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="图片 16"/>
+        <xdr:cNvPr id="31" name="图片 16"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACyxPQzHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAQAAAAAAAAAIABSgAQAAAAAQAAAMACHgFaAAAAczIAAAgIAADhAAAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACyxPQzHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAQAAAAAAAAAIABSgAQAAAAAQAAAMACHgFaAAAAczIAAAgIAADhAAAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1450,12 +1468,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="图片 17"/>
+        <xdr:cNvPr id="30" name="图片 17"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADhLSbqHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAARAAAAAAAAAAABAAARAAAAAQAAAAADWwAAAAAA6TQAAP0FAABoAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADhLSbqHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAARAAAAAAAAAAABAAARAAAAAQAAAAADWwAAAAAA6TQAAP0FAABoAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1501,12 +1519,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="图片 18"/>
+        <xdr:cNvPr id="29" name="图片 18"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACOoOYWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAASAAAAAAAAAFUAoAASAAAAAAAAAMADvgLDAAAAQTcAAJQCAABnAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACOoOYWHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAASAAAAAAAAAFUAoAASAAAAAAAAAMADvgLDAAAAQTcAAJQCAABnAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1552,12 +1570,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="图片 19"/>
+        <xdr:cNvPr id="28" name="图片 19"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABK6vbiHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAATAAAAAAAAAJUAhwATAAAAAAAAAJUD7wKkAAAAPjoAAO8CAAAcAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABK6vbiHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAATAAAAAAAAAJUAhwATAAAAAAAAAJUD7wKkAAAAPjoAAO8CAAAcAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1603,12 +1621,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="图片 20"/>
+        <xdr:cNvPr id="27" name="图片 20"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACJtFuHHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAUAAAAAAAAAJUAxQAUAAAAAAAAAIADpQLwAAAADj0AAEgCAAANAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACJtFuHHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAUAAAAAAAAAJUAxQAUAAAAAAAAAIADpQLwAAAADj0AAEgCAAANAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1654,12 +1672,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="图片 21"/>
+        <xdr:cNvPr id="26" name="图片 21"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACI2nkgHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAVAAAAAAAAAAAB3gAVAAAAAAAAAFgDEgIOAQAAKUAAAHcBAACmAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACI2nkgHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAVAAAAAAAAAAAB3gAVAAAAAAAAAFgDEgIOAQAAKUAAAHcBAACmAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1705,12 +1723,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="图片2"/>
+        <xdr:cNvPr id="25" name="图片2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC2GLGmHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAWAAAAAAAAACsB3gAWAAAAAAAAAEADNAIOAQAAF0MAAKEBAAB3AQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC2GLGmHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAWAAAAAAAAACsB3gAWAAAAAAAAAEADNAIOAQAAF0MAAKEBAAB3AQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1756,12 +1774,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="图片 23"/>
+        <xdr:cNvPr id="24" name="图片 23"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB4xTF+HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAXAAAAAAAAAKsAxQAXAAAAAAAAABUDawLwAAAAjUUAAAICAACzAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB4xTF+HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAXAAAAAAAAAKsAxQAXAAAAAAAAABUDawLwAAAAjUUAAAICAACzAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1807,12 +1825,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="图片 24"/>
+        <xdr:cNvPr id="23" name="图片 24"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA/3Pf3HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAYAAAAAAAAAGsA3gAYAAAAAAAAAKsDvgIOAQAAMEgAAEkCAABJAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA/3Pf3HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAYAAAAAAAAAGsA3gAYAAAAAAAAAKsDvgIOAQAAMEgAAEkCAABJAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1858,12 +1876,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="图片 25"/>
+        <xdr:cNvPr id="22" name="图片 25"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABSod4IHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAZAAAAAAAAAGsA9gAaAAAAAAAAAAAA4wIsAQAAAEsAAFgCAACFAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABSod4IHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAZAAAAAAAAAGsA9gAaAAAAAAAAAAAA4wIsAQAAAEsAAFgCAACFAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1909,12 +1927,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="图片 26"/>
+        <xdr:cNvPr id="21" name="图片 26"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACPYBuOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAaAAAAAAAAAIAAKAEaAAAAAAAAAEADsgJoAQAA300AAOABAADvAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACPYBuOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAaAAAAAAAAAIAAKAEaAAAAAAAAAEADsgJoAQAA300AAOABAADvAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -1960,12 +1978,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="图片 27"/>
+        <xdr:cNvPr id="20" name="图片 27"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADCrlgMHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAbAAAAAAAAABUAAwEbAAAAAAAAAMAD1wI7AQAAZFAAADoCAACUAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADCrlgMHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAbAAAAAAAAABUAAwEbAAAAAAAAAMAD1wI7AQAAZFAAADoCAACUAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2011,12 +2029,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="图片 28"/>
+        <xdr:cNvPr id="19" name="图片 28"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABikVqHHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAcAAAAAAAAAOsAGwEcAAAAAAAAAGsDvgJZAQAAylMAAP4BAADCAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABikVqHHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAcAAAAAAAAAOsAGwEcAAAAAAAAAGsDvgJZAQAAylMAAP4BAADCAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2062,12 +2080,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="图片 29"/>
+        <xdr:cNvPr id="18" name="图片 29"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB9c+vdHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAdAAAAAAAAAKsANAEdAAAAAAAAAJUD4wJ3AQAAbVYAAA0CAAANAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB9c+vdHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAdAAAAAAAAAKsANAEdAAAAAAAAAJUD4wJ3AQAAbVYAAA0CAAANAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2113,12 +2131,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="图片 30"/>
+        <xdr:cNvPr id="17" name="图片 30"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADGVx75HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAeAAAAAAAAAIAATQEeAAAAAAAAAGsD1wKWAQAAH1kAAN8BAAANAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADGVx75HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAeAAAAAAAAAIAATQEeAAAAAAAAAGsD1wKWAQAAH1kAAN8BAAANAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2164,12 +2182,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="图片 31"/>
+        <xdr:cNvPr id="16" name="图片 31"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABImbwnHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAfAAAAAAAAAIAATQEfAAAAAAAAAJUDmQKWAQAA71sAAJQBAAArAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABImbwnHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAfAAAAAAAAAIAATQEfAAAAAAAAAJUDmQKWAQAA71sAAJQBAAArAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2215,12 +2233,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="图片 32"/>
+        <xdr:cNvPr id="15" name="图片 32"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACTVH1MHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAgAAAAAAAAAGsA9gAgAAAAAAAAANUDvgIsAQAAsF4AACsCAABnAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACTVH1MHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAgAAAAAAAAAGsA9gAgAAAAAAAAANUDvgIsAQAAsF4AACsCAABnAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2266,12 +2284,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="图片 33"/>
+        <xdr:cNvPr id="14" name="图片 33"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAj+bdtHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAhAAAAAAAAAAABKAEhAAAAAAAAACsDmQJoAQAA6WEAAMIBAACGAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeAAAAAEAAABAAAAAAAAAAAAAAABaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAPAAAAAQAAACMAAAAjAAAAIwAAAB4AAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAj+bdtHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAhAAAAAAAAAAABKAEhAAAAAAAAACsDmQJoAQAA6WEAAMIBAACGAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2317,12 +2335,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="图片1"/>
+        <xdr:cNvPr id="13" name="图片1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC+b/ubHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAiAAAAAAAAAKsAAAEiAAAAAAAAAEAD1AI4AQAAfWQAADoCAADRAQAAAAAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC+b/ubHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAiAAAAAAAAAKsAAAEiAAAAAAAAAEAD1AI4AQAAfWQAADoCAADRAQAAAAAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2368,12 +2386,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="图片3"/>
+        <xdr:cNvPr id="12" name="图片3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAjAAAAAAAAAKsADAEjAAAAAAAAAFUDsAJGAQAATWcAAAACAADgAQAAAAAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAjAAAAAAAAAKsADAEjAAAAAAAAAFUDsAJGAQAATWcAAAACAADgAQAAAAAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2419,12 +2437,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="图片4"/>
+        <xdr:cNvPr id="11" name="图片4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABgqIUCHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAkAAAAAAAAAKsAAAEkAAAAAAAAAGsDrwI4AQAAHWoAAA0CAADvAQAAAAAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABgqIUCHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAkAAAAAAAAAKsAAAEkAAAAAAAAAGsDrwI4AQAAHWoAAA0CAADvAQAAAAAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2470,12 +2488,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="图片5"/>
+        <xdr:cNvPr id="10" name="图片5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC2GLGmHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAlAAAAAAAAAKsAJQElAAAAAAAAAGsDEwNlAQAAHW0AAFkCAACzAgAAAAAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC2GLGmHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAlAAAAAAAAAKsAJQElAAAAAAAAAGsDEwNlAQAAHW0AAFkCAACzAgAAAAAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2521,12 +2539,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="图片6"/>
+        <xdr:cNvPr id="9" name="图片6"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAmAAAAAAAAANUAcAEmAAAAAAAAAMADyQLAAQAA+HAAAKQBAAANAgAAAAAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAmAAAAAAAAANUAcAEmAAAAAAAAAMADyQLAAQAA+HAAAKQBAAANAgAAAAAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2572,12 +2590,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="图片7"/>
+        <xdr:cNvPr id="8" name="图片7"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAnAAAAAAAAANUAPQEnAAAAAAAAAHwDqwKCAQAAyHMAAL4BAADdAQAAAAAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAnAAAAAAAAANUAPQEnAAAAAAAAAHwDqwKCAQAAyHMAAL4BAADdAQAAAAAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2623,12 +2641,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="图片8"/>
+        <xdr:cNvPr id="7" name="图片8"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAApAAAAAAAAAKsAqwAqAAAAAAAAABUA1gLQAAAASnkAAKQCAABnAgAAAAAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAApAAAAAAAAAKsAqwAqAAAAAAAAABUA1gLQAAAASnkAAKQCAABnAgAAAAAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2674,12 +2692,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片9"/>
+        <xdr:cNvPr id="6" name="图片9"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADIifkYHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAqAAAAAAAAAPIAAAAqAAAAAAAAAEcD5AMAAAAATHwAAL0EAACkAQAAAAAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADIifkYHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAqAAAAAAAAAPIAAAAqAAAAAAAAAEcD5AMAAAAATHwAAL0EAACkAQAAAAAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2725,12 +2743,12 @@
     </xdr:to>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片10"/>
+        <xdr:cNvPr id="5" name="图片10"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAArAAAAAAAAANUAegArAAAAAQAAAAADAwCVAAAACH8AAFMEAACGAQAAAAAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAArAAAAAAAAANUAegArAAAAAQAAAAADAwCVAAAACH8AAFMEAACGAQAAAAAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2745,6 +2763,159 @@
         <a:xfrm>
           <a:off x="94615" y="20650200"/>
           <a:ext cx="702945" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>254635</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>415925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic macro="">
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+          <a:extLst>
+            <a:ext uri="smNativeData">
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAsAAAAAAAAANUASQEsAAAAAAAAAKQDngKRAQAA2IEAAJ8BAAD5AQAAAAAAAA=="/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="254635" y="21107400"/>
+          <a:ext cx="263525" cy="320675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>263525</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>568325</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic macro="">
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+          <a:extLst>
+            <a:ext uri="smNativeData">
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAtAAAAAAAAAEAAVQEuAAAAAAAAAAAA3wKfAQAAP4QAAOABAACjAgAAAAAAAA=="/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="263525" y="21497925"/>
+          <a:ext cx="304800" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>245110</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>511810</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic macro="">
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+          <a:extLst>
+            <a:ext uri="smNativeData">
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK8BAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAAAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAuAAAAAAAAAGsBPQEuAAAAAAAAACsDlgKCAQAA4YcAAKQBAAA7AQAAAAAAAA=="/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="245110" y="22088475"/>
+          <a:ext cx="266700" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2786,7 +2957,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABNAEEAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAACIAjAABAAAAAAAAAMkDwANpAQAA7AQAAEEIAADXDAAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABNAEEAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAACIAjAABAAAAAAAAAMkDwANpAQAA7AQAAEEIAADXDAAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2837,7 +3008,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAC0ALwACAAAAAAAAANMD9wN5AAAADBMAAL8JAAARCwAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAC0ALwACAAAAAAAAANMD9wN5AAAADBMAAL8JAAARCwAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2888,7 +3059,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAM4AAAADAAAAAQAAAEYDBgAAAAAA0CAAAF4KAACoBgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAM4AAAADAAAAAQAAAEYDBgAAAAAA0CAAAF4KAACoBgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2944,7 +3115,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABHup1/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAANsAeQABAAAAAAAAAD8DxgNJAQAAVAMAAPkIAACkAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAABHup1/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAABAAAAAAAAANsAeQABAAAAAAAAAD8DxgNJAQAAVAMAAPkIAACkAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -2995,7 +3166,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAMUAeQACAAAAAAAAABQDpANJAQAAAwYAAJ0IAACVAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAACAAAAAAAAAMUAeQACAAAAAAAAABQDpANJAQAAAwYAAJ0IAACVAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3046,7 +3217,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAJkATQADAAAAAAAAACoD9wPRAAAAowgAAPcJAADCAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAADAAAAAAAAAJkATQADAAAAAAAAACoD9wPRAAAAowgAAPcJAADCAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3097,7 +3268,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA8GCAkHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAJkAlQAEAAAAAAAAACoDgwOVAQAAYQsAAPcHAADCAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA8GCAkHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAEAAAAAAAAAJkAlQAEAAAAAAAAACoDgwOVAQAAYQsAAPcHAADCAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3148,7 +3319,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACGNUhOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAJkAmgAFAAAAAAAAAD8DjgOjAQAAHw4AAAcIAADRAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACGNUhOHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAFAAAAAAAAAJkAmgAFAAAAAAAAAD8DjgOjAQAAHw4AAAcIAADRAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3199,7 +3370,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAANsA0gAGAAAAAAAAAIEDaAM7AgAAChEAAAgHAADRAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAGAAAAAAAAANsA0gAGAAAAAAAAAIEDaAM7AgAAChEAAAgHAADRAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3250,7 +3421,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADYzLT/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAMUAlQAHAAAAAAAAAGsDqgOVAQAAuRMAAGEIAADRAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAADYzLT/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAAAAAAAMUAlQAHAAAAAAAAAGsDqgOVAQAAuRMAAGEIAADRAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3301,7 +3472,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB3m21HHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAANsAqwAIAAAAAAAAACoDlAPRAQAAhhYAAOkHAACVAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAB3m21HHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAIAAAAAAAAANsAqwAIAAAAAAAAACoDlAPRAQAAhhYAAOkHAACVAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3352,7 +3523,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAsq4VjHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIMAzAAJAAAAAAAAAFUDfgMrAgAACBkAAFQHAADvAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAsq4VjHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAAAAAAAIMAzAAJAAAAAAAAAFUDfgMrAgAACBkAAFQHAADvAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3403,7 +3574,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAHAAYAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAANsAsQAKAAAAAAAAAD8DfgPhAQAAAhwAAJ4HAACkAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAHAAYAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAKAAAAAAAAANsAsQAKAAAAAAAAAD8DfgPhAQAAAhwAAJ4HAACkAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3454,7 +3625,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAAMUApgALAAAAAAAAAIEDeAPDAQAAsR4AAKsHAADgAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAALAAAAAAAAAMUApgALAAAAAAAAAIEDeAPDAQAAsR4AAKsHAADgAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3505,7 +3676,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA5l2ZBHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAANsAhAAMAAAAAAAAAGsDbQNnAQAAfiEAAOkHAADCAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAA5l2ZBHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAAAAAAANsAhAAMAAAAAAAAAGsDbQNnAQAAfiEAAOkHAADCAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3556,7 +3727,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAG0AzAANAAAAAAAAAD8DGgMrAgAA8SMAAEQGAADvAQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAANAAAAAAAAAG0AzAANAAAAAAAAAD8DGgMrAgAA8SMAAEQGAADvAQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3607,7 +3778,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAFgAmgAOAAAAAAAAAGsDYgOjAQAAoCYAAI8HAAAcAgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAOAAAAAAAAAFgAmgAOAAAAAAAAAGsDYgOjAQAAoCYAAI8HAAAcAgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3658,7 +3829,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACqmnb/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAABQAAABYADwAOAAAACgAAAMUAAwEUMgAA9yAAAIYUAAD0BQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAACqmnb/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAMAAAABQAAABYADwAOAAAACgAAAMUAAwEUMgAA9yAAAIYUAAD0BQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3709,7 +3880,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC7q4v/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAABQAAAOEBDwAMAAAACgAAABYAuwEUMgAA+BkAADoVAAD/BgAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAC7q4v/HgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAJAAAABQAAAOEBDwAMAAAACgAAABYAuwEUMgAA+BkAADoVAAD/BgAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -3760,7 +3931,7 @@
           <a:picLocks noChangeAspect="1"/>
           <a:extLst>
             <a:ext uri="smNativeData">
-              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_rugfZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAABQAAAJACPQAJAAAACgAAAOEBtwBBMgAA9BQAAA4UAAAEBQAAAQAAAA=="/>
+              <pm:smNativeData xmlns:pm="smNativeData" val="SMDATA_15_lGElZBMAAAAlAAAAEQAAAK0AAAAAkAAAAEgAAACQAAAASAAAAAAAAAAAAAAAAAAAAAEAAABQAAAAAAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8AAAAAAADgPwAAAAAAAOA/AAAAAAAA4D8CAAAAjAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZAAAAAEAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAFAAAADwAAAAAAAAAAAAAAAAAAAAUAAAAAQAAABQAAAAUAAAAFAAAAAEAAAAAAAAAZAAAAGQAAAAAAAAAZAAAAGQAAAAVAAAAYAAAAAAAAAAAAAAADwAAACADAAAAAAAAAAAAAAEAAACgMgAAVgcAAKr4//8BAAAAf39/AAEAAABkAAAAAAAAABQAAABAHwAAAAAAACYAAAAAAAAAwOD//wAAAAAmAAAAZAAAABYAAABMAAAAAAAAAAAAAAAEAAAAAAAAAAEAAAB/f38AAAAAACgAAAAoAAAAZAAAAGQAAAAAAAAAzMzMAAAAAABQAAAAUAAAAGQAAABkAAAAAAAAAAcAAAA4AAAAAAAAAAAAAAAAAAAA////AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABkAAAAZAAAAAEAAAAjAAAABAAAAGQAAAAXAAAAFAAAAAAAAAAAAAAA/38AAP9/AAAAAAAACQAAAAQAAAAAAAAAHgAAAGgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAnAAAQJwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAAAMDA/wAAAAAAZAAAADIAAAAAAAAAZAAAAAAAAAB/f38ACgAAACIAAAAYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAJAAAACQAAAAAAAAABwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH9/fwAlAAAAWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPwAAAAAAAACghgEAAAAAAAAAAAAAAAAADAAAAAEAAAAAAAAAAAAAAAAAAAAhAAAAMAAAACwAAAAHAAAABQAAAJACPQAJAAAACgAAAOEBtwBBMgAA9BQAAA4UAAAEBQAAAQAAAA=="/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPicPr>
@@ -4052,8 +4223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:XFD112"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="C38" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.55"/>
@@ -11199,9 +11370,36 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="36" customHeight="1"/>
-    <row r="46" spans="1:1" ht="36" customHeight="1"/>
-    <row r="47" spans="1:1" ht="36" customHeight="1"/>
+    <row r="45" spans="2:5" ht="36" customHeight="1">
+      <c r="B45" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="36" customHeight="1">
+      <c r="B46" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="36" customHeight="1">
+      <c r="B47" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="48" spans="1:1" ht="36" customHeight="1"/>
     <row r="49" spans="1:1" ht="36" customHeight="1"/>
     <row r="50" spans="1:1" ht="36" customHeight="1"/>
@@ -11271,7 +11469,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1679812782" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1680171412" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -11280,17 +11478,17 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1679812782" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1679812782" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1679812782" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1679812782" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1680171412" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1680171412" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1680171412" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1680171412" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <drawing r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1679812782" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1680171412" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -11318,32 +11516,32 @@
   <sheetData>
     <row r="1" spans="2:4" ht="57" customHeight="1">
       <c r="B1" s="5" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="180" customHeight="1">
       <c r="B2" s="6" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="155.25" customHeight="1">
       <c r="B3" s="6" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D3" s="6" t="n">
         <v>0</v>
@@ -11351,13 +11549,13 @@
     </row>
     <row r="4" spans="2:4" ht="138" customHeight="1">
       <c r="B4" s="6" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="60" customHeight="1"/>
@@ -11476,7 +11674,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1679812782" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1680171412" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -11485,17 +11683,17 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1679812782" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1679812782" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1679812782" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1679812782" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1680171412" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1680171412" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1680171412" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1680171412" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <drawing r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1679812782" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1680171412" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -11522,16 +11720,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="35.10" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="35.10" customHeight="1">
@@ -11729,7 +11927,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1679812782" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1680171412" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -11738,17 +11936,17 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1679812782" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1679812782" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1679812782" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1679812782" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1680171412" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1680171412" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1680171412" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1680171412" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <drawing r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1679812782" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1680171412" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>